<commit_message>
ADD: new intent and text to answer
</commit_message>
<xml_diff>
--- a/train_tools/qna/train_data.xlsx
+++ b/train_tools/qna/train_data.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kei/PycharmProjects/first_chatbot/train_tools/qna/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\Chatbot_Intent\train_tools\qna\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A853BDA-43A5-AE4C-916E-BDA6CC036CF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21600" yWindow="-8880" windowWidth="21600" windowHeight="20940" xr2:uid="{91B3E3B2-3B68-0C4C-B8EF-7A84BAE2F665}"/>
+    <workbookView xWindow="-21600" yWindow="-8880" windowWidth="21600" windowHeight="20940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>개체명(NER)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,56 +75,44 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B_FOOD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{B_FOOD} 주문 처리 완료되었습니다. 
-주문해주셔서 감사합니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{B_FOOD} 주문할게요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>예약</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>B_DT,B_TI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{B_DT} 예약</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{B_DT}에 예약 접수 되었습니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>욕설</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>욕하면 나빠요 ㅠ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>{B_FOOD} 주문 처리 감사!!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://i.imgur.com/UluUFMp.jpg</t>
+    <t>만남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[경고]
+상대방이 갑작스러운 만남을
+요구할 경우에는 항상 조심하세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[경고]
+상대방이 갑작스러운 금전적
+요구할 경우에는 항상 조심하세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[경고]
+상대방과 나를 위해 욕설 사용은 자제해주세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -530,22 +517,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B4CC4D-BBB6-C948-A332-3C0CB96286D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="1" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23.44140625" customWidth="1"/>
+    <col min="4" max="4" width="24.109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -562,7 +549,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="38">
+    <row r="2" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -572,80 +559,51 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>20</v>
-      </c>
+      <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="38">
+    <row r="3" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>13</v>
+      </c>
+      <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5" ht="57">
+    <row r="4" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="19">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="D6" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="38">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="3" t="s">
+    <row r="7" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="19">
-      <c r="A7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{0E9BA614-0B84-764C-9F33-CC800C3C4E3B}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{F3941D0C-1C04-7A44-906E-8CC02273961F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
FIX: text of answer another intent
</commit_message>
<xml_diff>
--- a/train_tools/qna/train_data.xlsx
+++ b/train_tools/qna/train_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -19,20 +19,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>개체명(NER)</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,44 +59,40 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>반가워요</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주문</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>예약</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>욕설</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>만남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금전</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[경고]
+상대방이 갑작스러운 금전적
+요구할 경우에는 항상 조심하세요!</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[경고]
+상대방과 나를 위해 욕설 사용은 자제해주세요.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{B_DT} 만남</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B_DT,B_TI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>[경고]
 상대방이 갑작스러운 만남을
 요구할 경우에는 항상 조심하세요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>금전</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[경고]
-상대방이 갑작스러운 금전적
-요구할 경우에는 항상 조심하세요!</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[경고]
-상대방과 나를 위해 욕설 사용은 자제해주세요.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -187,7 +175,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -201,6 +189,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -521,7 +518,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="17.25" x14ac:dyDescent="0.3"/>
@@ -563,43 +560,40 @@
     </row>
     <row r="3" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="69" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:5" ht="51.75" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D7" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>